<commit_message>
Archivo Configuraciones para proposito y prioritarios, 1ra parte de correcciones en embalse
</commit_message>
<xml_diff>
--- a/php/archivo_excel.xlsx
+++ b/php/archivo_excel.xlsx
@@ -7,7 +7,8 @@
     <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Ingresar Año" sheetId="1" r:id="rId4"/>
+    <sheet name="2001" sheetId="1" r:id="rId4"/>
+    <sheet name="2012" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -363,7 +364,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -380,6 +381,596 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>210.008</v>
+      </c>
+      <c r="B2">
+        <v>1286.95</v>
+      </c>
+      <c r="C2">
+        <v>53.88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>210.01</v>
+      </c>
+      <c r="B3">
+        <v>1288.602</v>
+      </c>
+      <c r="C3">
+        <v>54.0316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>210.02</v>
+      </c>
+      <c r="B4">
+        <v>1290.254</v>
+      </c>
+      <c r="C4">
+        <v>54.1832</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>210.03</v>
+      </c>
+      <c r="B5">
+        <v>1291.906</v>
+      </c>
+      <c r="C5">
+        <v>54.3348</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>210.04</v>
+      </c>
+      <c r="B6">
+        <v>1293.559</v>
+      </c>
+      <c r="C6">
+        <v>54.4864</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>210.05</v>
+      </c>
+      <c r="B7">
+        <v>1295.211</v>
+      </c>
+      <c r="C7">
+        <v>54.638</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>210.06</v>
+      </c>
+      <c r="B8">
+        <v>1296.863</v>
+      </c>
+      <c r="C8">
+        <v>54.7896</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>210.07</v>
+      </c>
+      <c r="B9">
+        <v>1298.515</v>
+      </c>
+      <c r="C9">
+        <v>54.9412</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>210.08</v>
+      </c>
+      <c r="B10">
+        <v>1300.168</v>
+      </c>
+      <c r="C10">
+        <v>55.0928</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>210.09</v>
+      </c>
+      <c r="B11">
+        <v>1301.82</v>
+      </c>
+      <c r="C11">
+        <v>55.2444</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>210.1</v>
+      </c>
+      <c r="B12">
+        <v>1303.472</v>
+      </c>
+      <c r="C12">
+        <v>55.396</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>210.11</v>
+      </c>
+      <c r="B13">
+        <v>1305.124</v>
+      </c>
+      <c r="C13">
+        <v>55.5476</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>210.12</v>
+      </c>
+      <c r="B14">
+        <v>1306.776</v>
+      </c>
+      <c r="C14">
+        <v>55.6992</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>210.13</v>
+      </c>
+      <c r="B15">
+        <v>1308.429</v>
+      </c>
+      <c r="C15">
+        <v>55.8508</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>210.14</v>
+      </c>
+      <c r="B16">
+        <v>1310.081</v>
+      </c>
+      <c r="C16">
+        <v>56.0024</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>210.15</v>
+      </c>
+      <c r="B17">
+        <v>1311.733</v>
+      </c>
+      <c r="C17">
+        <v>56.154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>210.16</v>
+      </c>
+      <c r="B18">
+        <v>1313.385</v>
+      </c>
+      <c r="C18">
+        <v>56.3056</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>210.17</v>
+      </c>
+      <c r="B19">
+        <v>1315.037</v>
+      </c>
+      <c r="C19">
+        <v>56.4572</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>210.18</v>
+      </c>
+      <c r="B20">
+        <v>1316.69</v>
+      </c>
+      <c r="C20">
+        <v>56.6088</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>210.19</v>
+      </c>
+      <c r="B21">
+        <v>1318.342</v>
+      </c>
+      <c r="C21">
+        <v>56.7604</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>210.2</v>
+      </c>
+      <c r="B22">
+        <v>1319.994</v>
+      </c>
+      <c r="C22">
+        <v>56.912</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>210.21</v>
+      </c>
+      <c r="B23">
+        <v>1321.646</v>
+      </c>
+      <c r="C23">
+        <v>57.0636</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>210.22</v>
+      </c>
+      <c r="B24">
+        <v>1323.298</v>
+      </c>
+      <c r="C24">
+        <v>57.2152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>210.23</v>
+      </c>
+      <c r="B25">
+        <v>1324.951</v>
+      </c>
+      <c r="C25">
+        <v>57.3668</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>210.24</v>
+      </c>
+      <c r="B26">
+        <v>1326.603</v>
+      </c>
+      <c r="C26">
+        <v>57.5184</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>210.25</v>
+      </c>
+      <c r="B27">
+        <v>1328.255</v>
+      </c>
+      <c r="C27">
+        <v>57.67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>210.26</v>
+      </c>
+      <c r="B28">
+        <v>1329.907</v>
+      </c>
+      <c r="C28">
+        <v>57.8216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>210.27</v>
+      </c>
+      <c r="B29">
+        <v>1331.559</v>
+      </c>
+      <c r="C29">
+        <v>57.9732</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>210.28</v>
+      </c>
+      <c r="B30">
+        <v>1333.212</v>
+      </c>
+      <c r="C30">
+        <v>58.1248</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>210.29</v>
+      </c>
+      <c r="B31">
+        <v>1334.864</v>
+      </c>
+      <c r="C31">
+        <v>58.2764</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>210.3</v>
+      </c>
+      <c r="B2">
+        <v>1336.516</v>
+      </c>
+      <c r="C2">
+        <v>58.428</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>210.31</v>
+      </c>
+      <c r="B3">
+        <v>1338.168</v>
+      </c>
+      <c r="C3">
+        <v>58.5796</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>210.32</v>
+      </c>
+      <c r="B4">
+        <v>1339.82</v>
+      </c>
+      <c r="C4">
+        <v>58.7312</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>210.33</v>
+      </c>
+      <c r="B5">
+        <v>1341.473</v>
+      </c>
+      <c r="C5">
+        <v>58.8828</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>210.34</v>
+      </c>
+      <c r="B6">
+        <v>1343.125</v>
+      </c>
+      <c r="C6">
+        <v>59.0344</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>210.35</v>
+      </c>
+      <c r="B7">
+        <v>1344.777</v>
+      </c>
+      <c r="C7">
+        <v>59.186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>210.36</v>
+      </c>
+      <c r="B8">
+        <v>1346.429</v>
+      </c>
+      <c r="C8">
+        <v>59.3376</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>210.37</v>
+      </c>
+      <c r="B9">
+        <v>1348.081</v>
+      </c>
+      <c r="C9">
+        <v>59.4892</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>210.38</v>
+      </c>
+      <c r="B10">
+        <v>1349.734</v>
+      </c>
+      <c r="C10">
+        <v>59.6408</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>210.39</v>
+      </c>
+      <c r="B11">
+        <v>1351.386</v>
+      </c>
+      <c r="C11">
+        <v>59.7924</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>210.4</v>
+      </c>
+      <c r="B12">
+        <v>1353.038</v>
+      </c>
+      <c r="C12">
+        <v>59.944</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>210.41</v>
+      </c>
+      <c r="B13">
+        <v>1354.69</v>
+      </c>
+      <c r="C13">
+        <v>60.0956</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>210.42</v>
+      </c>
+      <c r="B14">
+        <v>1356.342</v>
+      </c>
+      <c r="C14">
+        <v>60.2472</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>210.43</v>
+      </c>
+      <c r="B15">
+        <v>1357.995</v>
+      </c>
+      <c r="C15">
+        <v>60.3988</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>210.44</v>
+      </c>
+      <c r="B16">
+        <v>1359.647</v>
+      </c>
+      <c r="C16">
+        <v>60.5504</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>210.45</v>
+      </c>
+      <c r="B17">
+        <v>1361.299</v>
+      </c>
+      <c r="C17">
+        <v>60.702</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>210.46</v>
+      </c>
+      <c r="B18">
+        <v>1362.951</v>
+      </c>
+      <c r="C18">
+        <v>60.8536</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>210.47</v>
+      </c>
+      <c r="B19">
+        <v>1364.603</v>
+      </c>
+      <c r="C19">
+        <v>61.0052</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>210.48</v>
+      </c>
+      <c r="B20">
+        <v>1366.256</v>
+      </c>
+      <c r="C20">
+        <v>61.1568</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>210.49</v>
+      </c>
+      <c r="B21">
+        <v>1367.908</v>
+      </c>
+      <c r="C21">
+        <v>61.3084</v>
       </c>
     </row>
   </sheetData>

</xml_diff>